<commit_message>
add more "a" data
</commit_message>
<xml_diff>
--- a/historical/data/data.xlsx
+++ b/historical/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiansp/Learning/linguistics/historical/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB46D6-02A8-DF47-8124-9FCF3D671966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF97172-1735-8445-80DF-07DD940B4211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="24700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="888">
   <si>
     <t xml:space="preserve">baby						</t>
   </si>
@@ -2408,6 +2408,282 @@
   </si>
   <si>
     <t>automne</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Erle</t>
+  </si>
+  <si>
+    <t>Alge</t>
+  </si>
+  <si>
+    <t>verärgert, wütend</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Antwort, Beantwortung</t>
+  </si>
+  <si>
+    <t>Ameise</t>
+  </si>
+  <si>
+    <t>Apfel</t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>Pfeil</t>
+  </si>
+  <si>
+    <t>Esche</t>
+  </si>
+  <si>
+    <t>beschämt</t>
+  </si>
+  <si>
+    <t>Asche</t>
+  </si>
+  <si>
+    <t>fragen, bitten, enfragen</t>
+  </si>
+  <si>
+    <t>Herbst, Spätjahr</t>
+  </si>
+  <si>
+    <t>wecken, erwachen, erwecken</t>
+  </si>
+  <si>
+    <t>Axt, Beil</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>τσεκούρι, πέλεκυς, είδος μουσικής</t>
+  </si>
+  <si>
+    <t>κλήθρα</t>
+  </si>
+  <si>
+    <t>άλγη</t>
+  </si>
+  <si>
+    <t>θυμωμένος</t>
+  </si>
+  <si>
+    <t>ζώο</t>
+  </si>
+  <si>
+    <t>απάντηση</t>
+  </si>
+  <si>
+    <t>μυρμήγκι, μύρμιξ</t>
+  </si>
+  <si>
+    <t>μήλο</t>
+  </si>
+  <si>
+    <t>μπράτσο</t>
+  </si>
+  <si>
+    <t>βέλος</t>
+  </si>
+  <si>
+    <t>φλαμουριά</t>
+  </si>
+  <si>
+    <t>elm</t>
+  </si>
+  <si>
+    <t>ντροπιασμένος</t>
+  </si>
+  <si>
+    <t>τέφρα, στάκτη, μελιά</t>
+  </si>
+  <si>
+    <t>παρακαλώ, ζητώ</t>
+  </si>
+  <si>
+    <t>φθινόπωρο</t>
+  </si>
+  <si>
+    <t>αφυπνίζω</t>
+  </si>
+  <si>
+    <t>GkTr</t>
+  </si>
+  <si>
+    <t>klithra</t>
+  </si>
+  <si>
+    <t>algi</t>
+  </si>
+  <si>
+    <t>zoo</t>
+  </si>
+  <si>
+    <t>apantisi</t>
+  </si>
+  <si>
+    <t>thimomenos</t>
+  </si>
+  <si>
+    <t>mirmigki, myrmix</t>
+  </si>
+  <si>
+    <t>milo</t>
+  </si>
+  <si>
+    <t>bratso</t>
+  </si>
+  <si>
+    <t>velos</t>
+  </si>
+  <si>
+    <t>flamouria</t>
+  </si>
+  <si>
+    <t>ndropiasmenos</t>
+  </si>
+  <si>
+    <t>tefra, stakti, melia</t>
+  </si>
+  <si>
+    <t>parakalo, zito</t>
+  </si>
+  <si>
+    <t>fthinoporo</t>
+  </si>
+  <si>
+    <t>tsekouri, pelekys, eidhos mousikis</t>
+  </si>
+  <si>
+    <t>afypnizo</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>GujTr</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>HndTr</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t>Icelandic</t>
+  </si>
+  <si>
+    <t>Irish</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Kazakh</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Kyrgyz</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Latvian</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Burmese</t>
+  </si>
+  <si>
+    <t>Nepali</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Sanskrit</t>
+  </si>
+  <si>
+    <t>Scots Gaelic</t>
+  </si>
+  <si>
+    <t>Serbian</t>
+  </si>
+  <si>
+    <t>Sinhala</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>Slovenian</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Tajik</t>
+  </si>
+  <si>
+    <t>Tatar</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>Turkmen</t>
+  </si>
+  <si>
+    <t>Ukranian</t>
+  </si>
+  <si>
+    <t>Uyghur</t>
+  </si>
+  <si>
+    <t>Uzbek</t>
+  </si>
+  <si>
+    <t>Welsh</t>
   </si>
 </sst>
 </file>
@@ -3251,13 +3527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S505"/>
+  <dimension ref="A1:BJ506"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3279,9 +3555,12 @@
     <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>477</v>
       </c>
@@ -3339,8 +3618,137 @@
       <c r="S1" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" t="s">
+        <v>796</v>
+      </c>
+      <c r="U1" t="s">
+        <v>813</v>
+      </c>
+      <c r="V1" t="s">
+        <v>831</v>
+      </c>
+      <c r="W1" t="s">
+        <v>848</v>
+      </c>
+      <c r="X1" t="s">
+        <v>849</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>850</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>851</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>852</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>853</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>854</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>855</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>856</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>857</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>858</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>859</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>860</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>861</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>862</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>863</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>864</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>865</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>866</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>867</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>868</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>869</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>870</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>871</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>872</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>873</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>874</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>875</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>876</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>877</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>878</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>879</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>880</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>881</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>882</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>883</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>884</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>885</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>886</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>478</v>
       </c>
@@ -3398,8 +3806,17 @@
       <c r="S2" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" t="s">
+        <v>496</v>
+      </c>
+      <c r="U2" t="s">
+        <v>496</v>
+      </c>
+      <c r="V2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>479</v>
       </c>
@@ -3451,8 +3868,17 @@
       <c r="S3" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>797</v>
+      </c>
+      <c r="U3" t="s">
+        <v>815</v>
+      </c>
+      <c r="V3" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>492</v>
       </c>
@@ -3510,8 +3936,17 @@
       <c r="S4" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="T4" t="s">
+        <v>798</v>
+      </c>
+      <c r="U4" t="s">
+        <v>816</v>
+      </c>
+      <c r="V4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>480</v>
       </c>
@@ -3569,8 +4004,17 @@
       <c r="S5" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>799</v>
+      </c>
+      <c r="U5" t="s">
+        <v>817</v>
+      </c>
+      <c r="V5" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>481</v>
       </c>
@@ -3628,8 +4072,17 @@
       <c r="S6" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>800</v>
+      </c>
+      <c r="U6" t="s">
+        <v>818</v>
+      </c>
+      <c r="V6" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -3687,8 +4140,17 @@
       <c r="S7" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7" t="s">
+        <v>801</v>
+      </c>
+      <c r="U7" t="s">
+        <v>819</v>
+      </c>
+      <c r="V7" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>483</v>
       </c>
@@ -3746,8 +4208,17 @@
       <c r="S8" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>802</v>
+      </c>
+      <c r="U8" t="s">
+        <v>820</v>
+      </c>
+      <c r="V8" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>484</v>
       </c>
@@ -3805,8 +4276,17 @@
       <c r="S9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9" t="s">
+        <v>803</v>
+      </c>
+      <c r="U9" t="s">
+        <v>821</v>
+      </c>
+      <c r="V9" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>485</v>
       </c>
@@ -3864,8 +4344,17 @@
       <c r="S10" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>804</v>
+      </c>
+      <c r="U10" t="s">
+        <v>822</v>
+      </c>
+      <c r="V10" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>486</v>
       </c>
@@ -3923,8 +4412,17 @@
       <c r="S11" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11" t="s">
+        <v>805</v>
+      </c>
+      <c r="U11" t="s">
+        <v>823</v>
+      </c>
+      <c r="V11" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>509</v>
       </c>
@@ -3967,8 +4465,17 @@
       <c r="S12" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>806</v>
+      </c>
+      <c r="U12" t="s">
+        <v>824</v>
+      </c>
+      <c r="V12" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>487</v>
       </c>
@@ -4026,8 +4533,17 @@
       <c r="S13" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13" t="s">
+        <v>807</v>
+      </c>
+      <c r="U13" t="s">
+        <v>826</v>
+      </c>
+      <c r="V13" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>510</v>
       </c>
@@ -4085,8 +4601,17 @@
       <c r="S14" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>808</v>
+      </c>
+      <c r="U14" t="s">
+        <v>827</v>
+      </c>
+      <c r="V14" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>488</v>
       </c>
@@ -4144,8 +4669,17 @@
       <c r="S15" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>809</v>
+      </c>
+      <c r="U15" t="s">
+        <v>828</v>
+      </c>
+      <c r="V15" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>489</v>
       </c>
@@ -4203,8 +4737,17 @@
       <c r="S16" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16" t="s">
+        <v>810</v>
+      </c>
+      <c r="U16" t="s">
+        <v>829</v>
+      </c>
+      <c r="V16" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>490</v>
       </c>
@@ -4262,8 +4805,17 @@
       <c r="S17" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17" t="s">
+        <v>811</v>
+      </c>
+      <c r="U17" t="s">
+        <v>830</v>
+      </c>
+      <c r="V17" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>491</v>
       </c>
@@ -4321,73 +4873,82 @@
       <c r="S18" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>812</v>
+      </c>
+      <c r="U18" t="s">
+        <v>814</v>
+      </c>
+      <c r="V18" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -4931,1841 +5492,1846 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>825</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>647</v>
+        <v>217</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>218</v>
+        <v>647</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>493</v>
+        <v>280</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>281</v>
+        <v>493</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>603</v>
+        <v>337</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>338</v>
+        <v>603</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>605</v>
+        <v>353</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>354</v>
+        <v>605</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
         <v>476</v>
       </c>
     </row>

</xml_diff>